<commit_message>
Clean and reshape Census
</commit_message>
<xml_diff>
--- a/references/Data Catalog.xlsx
+++ b/references/Data Catalog.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="80">
   <si>
     <t>Outcome</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Median wages</t>
   </si>
   <si>
-    <t>2009-2017</t>
-  </si>
-  <si>
     <t>Main Dataset</t>
   </si>
   <si>
@@ -111,9 +108,6 @@
     <t>Quality of life</t>
   </si>
   <si>
-    <t>poverty status</t>
-  </si>
-  <si>
     <t>poverty status of families</t>
   </si>
   <si>
@@ -253,6 +247,24 @@
   </si>
   <si>
     <t>week of March 12, also gives Q1 and annual payroll. Gives it by SIC/NAICS, but we'll just download aggregate for zip code.</t>
+  </si>
+  <si>
+    <t>only for pop 25+, did not include 18-24</t>
+  </si>
+  <si>
+    <t>2012-2017</t>
+  </si>
+  <si>
+    <t>2010-2017</t>
+  </si>
+  <si>
+    <t>poverty status by educational attainment</t>
+  </si>
+  <si>
+    <t>poverty status by race</t>
+  </si>
+  <si>
+    <t>??</t>
   </si>
 </sst>
 </file>
@@ -596,11 +608,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B39" sqref="B39"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -626,7 +638,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>3</v>
@@ -635,10 +647,10 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -646,7 +658,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
@@ -661,10 +673,10 @@
         <v>8</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -672,7 +684,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -687,10 +699,10 @@
         <v>8</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -698,7 +710,7 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
@@ -713,10 +725,10 @@
         <v>8</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -724,19 +736,22 @@
         <v>11</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>12</v>
+        <v>76</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -744,99 +759,117 @@
         <v>11</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>76</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="D7" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>12</v>
+        <v>76</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>12</v>
+        <v>76</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>12</v>
+        <v>76</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E10" t="s">
         <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
+        <v>76</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -844,122 +877,137 @@
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E11" t="s">
         <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>12</v>
+        <v>76</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E12" t="s">
+        <v>10</v>
+      </c>
+      <c r="F12" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E13" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" t="s">
+        <v>75</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E12" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>27</v>
-      </c>
-      <c r="B13" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E13" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="D14" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E14" t="s">
         <v>10</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>76</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E15" t="s">
         <v>10</v>
       </c>
       <c r="F15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+        <v>76</v>
+      </c>
+      <c r="H15" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E16" t="s">
         <v>10</v>
       </c>
       <c r="F16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>36</v>
+        <v>76</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -967,25 +1015,25 @@
         <v>9</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E17" t="s">
         <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H17" t="s">
-        <v>71</v>
+        <v>34</v>
+      </c>
+      <c r="H17" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -993,25 +1041,25 @@
         <v>9</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E18" t="s">
         <v>10</v>
       </c>
       <c r="F18" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1019,25 +1067,25 @@
         <v>9</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="D19" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E19" t="s">
         <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="H19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1045,192 +1093,230 @@
         <v>9</v>
       </c>
       <c r="B20" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E20" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" t="s">
+        <v>76</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E21" t="s">
+        <v>10</v>
+      </c>
+      <c r="F21" t="s">
+        <v>76</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E20" t="s">
-        <v>10</v>
-      </c>
-      <c r="F20" t="s">
-        <v>12</v>
-      </c>
-      <c r="G20" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="H20" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>27</v>
-      </c>
-      <c r="B21" s="3" t="s">
+      <c r="D22" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E22" t="s">
+        <v>10</v>
+      </c>
+      <c r="F22" t="s">
+        <v>76</v>
+      </c>
+      <c r="G22" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="E21" t="s">
-        <v>10</v>
-      </c>
-      <c r="F21" t="s">
-        <v>12</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E22" t="s">
-        <v>10</v>
-      </c>
-      <c r="F22" t="s">
-        <v>12</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>53</v>
+      <c r="H22" s="3" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B23" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" t="s">
+        <v>10</v>
+      </c>
+      <c r="F23" t="s">
+        <v>76</v>
+      </c>
+      <c r="G23" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="3" t="s">
+      <c r="H23" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" t="s">
+        <v>10</v>
+      </c>
+      <c r="F24" t="s">
+        <v>76</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D23" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E23" t="s">
-        <v>10</v>
-      </c>
-      <c r="F23" t="s">
-        <v>12</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E24" t="s">
-        <v>10</v>
-      </c>
-      <c r="F24" t="s">
-        <v>12</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>57</v>
+      <c r="H24" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>26</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E25" t="s">
         <v>10</v>
       </c>
       <c r="F25" t="s">
-        <v>12</v>
+        <v>76</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="H25" t="s">
-        <v>71</v>
+        <v>55</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" t="s">
+        <v>10</v>
+      </c>
+      <c r="F26" t="s">
+        <v>76</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H26" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>60</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="D27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" t="s">
+        <v>10</v>
+      </c>
+      <c r="F27" t="s">
+        <v>76</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="3" t="s">
+      <c r="H27" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" t="s">
         <v>64</v>
       </c>
-      <c r="D26" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" t="s">
-        <v>10</v>
-      </c>
-      <c r="F26" t="s">
-        <v>12</v>
-      </c>
-      <c r="G26" s="3" t="s">
+      <c r="F28" t="s">
         <v>65</v>
       </c>
-      <c r="H26" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E27" t="s">
+      <c r="G28" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="F27" t="s">
-        <v>67</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1254,18 +1340,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>